<commit_message>
Actualización de Pruebas de Catálogos de Almacen
</commit_message>
<xml_diff>
--- a/Documentación/04 - Transición/ALMACEN - Pruebas de la Aplicación.xlsx
+++ b/Documentación/04 - Transición/ALMACEN - Pruebas de la Aplicación.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="9555" windowHeight="6720"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="9555" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="62">
   <si>
     <t>Catálogo de Familias</t>
   </si>
@@ -110,24 +110,15 @@
     <t>Incorrecto</t>
   </si>
   <si>
-    <t>No muestra el formulario para crear nuevo Producto</t>
-  </si>
-  <si>
     <t>Validar que se realice la búsqueda avanzada de Productos</t>
   </si>
   <si>
-    <t>Validar que en búsqueda avanzada se llene el campo de texto para mostrar un Producto</t>
-  </si>
-  <si>
     <t>Validar que en búsqueda avanzada se llene el campo de texto para mostrar una Marca</t>
   </si>
   <si>
     <t>Validar que se realice la búsqueda avanzada de Marcas</t>
   </si>
   <si>
-    <t>No muestra el formulario para buscar un Producto</t>
-  </si>
-  <si>
     <t>Validar que el botón Cancelar en Búsqueda Avanzada funcione correctamente</t>
   </si>
   <si>
@@ -173,17 +164,53 @@
     <t>Validar que en búsqueda avanzada se llene el campo de texto para mostrar una Familia</t>
   </si>
   <si>
-    <t xml:space="preserve">Validar que no muestre en Búsqueda Personalizada la lista de familias al teclar una no existente </t>
-  </si>
-  <si>
     <t>Error en Pantalla (no la muestra)</t>
+  </si>
+  <si>
+    <t>Si falta algún campo obligatorio no muestra un mensaje de error o de aviso</t>
+  </si>
+  <si>
+    <t>No muestra mensaje de confirmación</t>
+  </si>
+  <si>
+    <t>No muestra mensaje de error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validar que no muestre en Búsqueda Avanzada la lista de familias al teclar una no existente </t>
+  </si>
+  <si>
+    <t>Sólo se muestran algunos mensajes de confirmación y falta corregir tamaño de ventana</t>
+  </si>
+  <si>
+    <t>Sólo se muestran algunos mensajes de error al llenar algun campo de formulario y falta corregir tamaño de ventana</t>
+  </si>
+  <si>
+    <t>Si no se llena el campo muestra todas las subfamilias</t>
+  </si>
+  <si>
+    <t>Si no se llena el campo se muestran todas las familias</t>
+  </si>
+  <si>
+    <t>Al dar clic en botón Guardar, truena la aplicación</t>
+  </si>
+  <si>
+    <t>Validar que limpie campos con el botón Limpiar</t>
+  </si>
+  <si>
+    <t>Validar que en búsqueda avanzada se llenen los campos de texto para mostrar un Producto</t>
+  </si>
+  <si>
+    <t>Si no se llena el campo muestra todos los productos</t>
+  </si>
+  <si>
+    <t>Si no se llena el campo muestra todas las marcas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +229,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,15 +280,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -264,21 +302,37 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -577,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -590,20 +644,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -626,8 +680,8 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>52</v>
+      <c r="E5" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -640,10 +694,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E84"/>
+  <dimension ref="A2:E85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -656,20 +710,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -689,193 +743,253 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="25.5" customHeight="1">
-      <c r="A6" s="9"/>
+      <c r="D5" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29.25" customHeight="1">
+      <c r="A6" s="11"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="25.5" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="33" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="33" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="5" t="s">
-        <v>49</v>
+      <c r="A10" s="11"/>
+      <c r="B10" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" ht="32.25" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="5" t="s">
-        <v>50</v>
+      <c r="A11" s="11"/>
+      <c r="B11" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="5" t="s">
-        <v>51</v>
+      <c r="A12" s="11"/>
+      <c r="B12" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D12" s="14" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="30">
-      <c r="A13" s="9"/>
-      <c r="B13" s="5" t="s">
-        <v>36</v>
+      <c r="A13" s="11"/>
+      <c r="B13" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="30">
-      <c r="A15" s="9" t="s">
+      <c r="D14" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="47.25" customHeight="1">
+      <c r="A15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="9"/>
-      <c r="B16" s="11" t="s">
+      <c r="D15" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45">
+      <c r="A16" s="11"/>
+      <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D16" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="45">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D17" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="30">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D18" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="30">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D19" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="45">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:5" ht="30">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10" t="s">
+      <c r="A21" s="11"/>
+      <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D21" s="15"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1">
       <c r="A25" s="2" t="s">
@@ -895,156 +1009,212 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>39</v>
+      <c r="B26" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1">
-      <c r="A27" s="9"/>
+      <c r="D26" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" customHeight="1">
+      <c r="A27" s="11"/>
       <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="25.5" customHeight="1">
-      <c r="A28" s="9"/>
-      <c r="B28" s="4" t="s">
+      <c r="A28" s="11"/>
+      <c r="B28" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D28" s="14" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A29" s="9"/>
-      <c r="B29" s="5" t="s">
-        <v>42</v>
+      <c r="A29" s="11"/>
+      <c r="B29" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="33" customHeight="1">
-      <c r="A30" s="9"/>
-      <c r="B30" s="5" t="s">
-        <v>43</v>
+      <c r="A30" s="11"/>
+      <c r="B30" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="33" customHeight="1">
-      <c r="A31" s="9"/>
-      <c r="B31" s="5" t="s">
-        <v>44</v>
+      <c r="A31" s="11"/>
+      <c r="B31" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D31" s="14" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="32.25" customHeight="1">
-      <c r="A32" s="9"/>
-      <c r="B32" s="5" t="s">
-        <v>45</v>
+      <c r="A32" s="11"/>
+      <c r="B32" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="37.5" customHeight="1">
-      <c r="A33" s="9"/>
-      <c r="B33" s="5" t="s">
-        <v>46</v>
+      <c r="A33" s="11"/>
+      <c r="B33" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D33" s="14" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="30">
-      <c r="A34" s="9"/>
-      <c r="B34" s="5" t="s">
-        <v>36</v>
+      <c r="A34" s="11"/>
+      <c r="B34" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30">
-      <c r="A35" s="9"/>
-      <c r="B35" s="10" t="s">
+      <c r="A35" s="11"/>
+      <c r="B35" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:5" ht="30">
-      <c r="A36" s="9" t="s">
+      <c r="D35" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="50.25" customHeight="1">
+      <c r="A36" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="30">
-      <c r="A37" s="9"/>
-      <c r="B37" s="11" t="s">
+      <c r="D36" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="45">
+      <c r="A37" s="11"/>
+      <c r="B37" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D37" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="45">
-      <c r="A38" s="9"/>
-      <c r="B38" s="10" t="s">
+      <c r="A38" s="11"/>
+      <c r="B38" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D38" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="30">
-      <c r="A39" s="9"/>
-      <c r="B39" s="10" t="s">
+      <c r="A39" s="11"/>
+      <c r="B39" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D39" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="30">
-      <c r="A40" s="9"/>
-      <c r="B40" s="10" t="s">
+      <c r="A40" s="11"/>
+      <c r="B40" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D40" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="45">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1052,8 +1222,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="30">
-      <c r="A42" s="9"/>
-      <c r="B42" s="10" t="s">
+      <c r="A42" s="11"/>
+      <c r="B42" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1068,20 +1238,20 @@
       <c r="E43" s="12"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
     </row>
     <row r="45" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" spans="1:5" ht="18.75" customHeight="1">
       <c r="A46" s="2" t="s">
@@ -1101,168 +1271,221 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="30.75" customHeight="1">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>38</v>
+      <c r="B47" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1">
-      <c r="A48" s="9"/>
+      <c r="D47" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="30" customHeight="1">
+      <c r="A48" s="11"/>
       <c r="B48" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="25.5" customHeight="1">
-      <c r="A49" s="9"/>
-      <c r="B49" s="4" t="s">
+      <c r="D48" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="25.5" customHeight="1">
+      <c r="A49" s="11"/>
+      <c r="B49" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="31.5" customHeight="1">
-      <c r="A50" s="9"/>
-      <c r="B50" s="5" t="s">
-        <v>37</v>
+      <c r="D49" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="31.5" customHeight="1">
+      <c r="A50" s="11"/>
+      <c r="B50" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="33" customHeight="1">
-      <c r="A51" s="9"/>
-      <c r="B51" s="5" t="s">
-        <v>40</v>
+      <c r="D50" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="33" customHeight="1">
+      <c r="A51" s="11"/>
+      <c r="B51" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="33" customHeight="1">
-      <c r="A52" s="9"/>
-      <c r="B52" s="5" t="s">
-        <v>34</v>
+      <c r="D51" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="33" customHeight="1">
+      <c r="A52" s="11"/>
+      <c r="B52" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="32.25" customHeight="1">
-      <c r="A53" s="9"/>
-      <c r="B53" s="5" t="s">
-        <v>33</v>
+      <c r="D52" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="32.25" customHeight="1">
+      <c r="A53" s="11"/>
+      <c r="B53" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="36.75" customHeight="1">
-      <c r="A54" s="9"/>
-      <c r="B54" s="5" t="s">
-        <v>47</v>
+      <c r="D53" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="36.75" customHeight="1">
+      <c r="A54" s="11"/>
+      <c r="B54" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="30">
-      <c r="A55" s="9"/>
-      <c r="B55" s="5" t="s">
-        <v>36</v>
+      <c r="D54" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="30">
+      <c r="A55" s="11"/>
+      <c r="B55" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="30">
-      <c r="A56" s="9"/>
-      <c r="B56" s="10" t="s">
+      <c r="D55" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30">
+      <c r="A56" s="11"/>
+      <c r="B56" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="4"/>
-    </row>
-    <row r="57" spans="1:4" ht="30">
-      <c r="A57" s="9" t="s">
+      <c r="D56" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="60">
+      <c r="A57" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="30">
-      <c r="A58" s="9"/>
-      <c r="B58" s="11" t="s">
+      <c r="D57" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="45">
+      <c r="A58" s="11"/>
+      <c r="B58" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="45">
-      <c r="A59" s="9"/>
-      <c r="B59" s="10" t="s">
+      <c r="D58" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="45">
+      <c r="A59" s="11"/>
+      <c r="B59" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="30">
-      <c r="A60" s="9"/>
-      <c r="B60" s="10" t="s">
+      <c r="D59" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="11"/>
+      <c r="B60" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="30">
-      <c r="A61" s="9"/>
-      <c r="B61" s="10" t="s">
+      <c r="D60" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30">
+      <c r="A61" s="11"/>
+      <c r="B61" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="45">
-      <c r="A62" s="9" t="s">
+      <c r="D61" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="45">
+      <c r="A62" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30">
-      <c r="A63" s="9"/>
-      <c r="B63" s="10" t="s">
+    <row r="63" spans="1:5" ht="30">
+      <c r="A63" s="11"/>
+      <c r="B63" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -1270,20 +1493,20 @@
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
     </row>
     <row r="66" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
+      <c r="A66" s="10"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
     </row>
     <row r="67" spans="1:5" ht="18.75" customHeight="1">
       <c r="A67" s="2" t="s">
@@ -1303,207 +1526,260 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="25.5" customHeight="1">
-      <c r="A69" s="9"/>
+      <c r="D68" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="31.5" customHeight="1">
+      <c r="A69" s="11"/>
       <c r="B69" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="25.5" customHeight="1">
-      <c r="A70" s="9"/>
-      <c r="B70" s="4" t="s">
+      <c r="D69" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="33.75" customHeight="1">
+      <c r="A70" s="11"/>
+      <c r="B70" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D70" s="5"/>
+      <c r="E70" s="17" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="71" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A71" s="9"/>
-      <c r="B71" s="5" t="s">
+      <c r="A71" s="11"/>
+      <c r="B71" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E71" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="E71" s="17"/>
     </row>
     <row r="72" spans="1:5" ht="33" customHeight="1">
-      <c r="A72" s="9"/>
-      <c r="B72" s="5" t="s">
-        <v>41</v>
+      <c r="A72" s="11"/>
+      <c r="B72" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D72" s="14"/>
+      <c r="E72" s="17" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="73" spans="1:5" ht="33" customHeight="1">
-      <c r="A73" s="9"/>
-      <c r="B73" s="5" t="s">
-        <v>31</v>
+      <c r="A73" s="11"/>
+      <c r="B73" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E73" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="32.25" customHeight="1">
-      <c r="A74" s="9"/>
-      <c r="B74" s="5" t="s">
-        <v>32</v>
+      <c r="D73" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="17"/>
+    </row>
+    <row r="74" spans="1:5" ht="33" customHeight="1">
+      <c r="A74" s="11"/>
+      <c r="B74" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="39" customHeight="1">
-      <c r="A75" s="9"/>
-      <c r="B75" s="5" t="s">
-        <v>48</v>
+      <c r="D74" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="17"/>
+    </row>
+    <row r="75" spans="1:5" ht="32.25" customHeight="1">
+      <c r="A75" s="11"/>
+      <c r="B75" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E75" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="30">
-      <c r="A76" s="9"/>
-      <c r="B76" s="5" t="s">
-        <v>36</v>
+      <c r="D75" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="39" customHeight="1">
+      <c r="A76" s="11"/>
+      <c r="B76" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D76" s="4"/>
-      <c r="E76" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="D76" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="19"/>
     </row>
     <row r="77" spans="1:5" ht="30">
-      <c r="A77" s="9"/>
-      <c r="B77" s="10" t="s">
-        <v>11</v>
+      <c r="A77" s="11"/>
+      <c r="B77" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D77" s="4"/>
+      <c r="D77" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="17"/>
     </row>
     <row r="78" spans="1:5" ht="30">
-      <c r="A78" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>13</v>
+      <c r="A78" s="11"/>
+      <c r="B78" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="30">
-      <c r="A79" s="9"/>
-      <c r="B79" s="11" t="s">
-        <v>14</v>
+      <c r="D78" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="60">
+      <c r="A79" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D79" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="80" spans="1:5" ht="45">
-      <c r="A80" s="9"/>
-      <c r="B80" s="10" t="s">
-        <v>15</v>
+      <c r="A80" s="11"/>
+      <c r="B80" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" ht="30">
-      <c r="A81" s="9"/>
-      <c r="B81" s="10" t="s">
-        <v>16</v>
+      <c r="D80" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="45">
+      <c r="A81" s="11"/>
+      <c r="B81" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" ht="30">
-      <c r="A82" s="9"/>
-      <c r="B82" s="10" t="s">
-        <v>20</v>
+      <c r="D81" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="30">
+      <c r="A82" s="11"/>
+      <c r="B82" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" ht="45">
-      <c r="A83" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>22</v>
+      <c r="D82" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="30">
+      <c r="A83" s="11"/>
+      <c r="B83" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="30">
-      <c r="A84" s="9"/>
-      <c r="B84" s="10" t="s">
-        <v>23</v>
+      <c r="D83" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="45">
+      <c r="A84" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="85" spans="1:4" ht="30">
+      <c r="A85" s="11"/>
+      <c r="B85" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A65:E66"/>
-    <mergeCell ref="A68:A77"/>
-    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="A2:E3"/>
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A23:E24"/>
+    <mergeCell ref="A26:A35"/>
+    <mergeCell ref="A36:A40"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="A22:E22"/>
     <mergeCell ref="A44:E45"/>
     <mergeCell ref="A47:A56"/>
     <mergeCell ref="A57:A61"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A23:E24"/>
-    <mergeCell ref="A26:A35"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A2:E3"/>
-    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A65:E66"/>
+    <mergeCell ref="A68:A78"/>
+    <mergeCell ref="A79:A83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>